<commit_message>
lots of random commits?
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proba\IdeaProjects\Jinseo_Bot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D2D43F-43BC-4038-8027-2904E03EE121}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708ADFE4-39E8-447A-A883-133605563608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3A43137D-FF13-441C-8D27-8175FD9C3C57}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{3A43137D-FF13-441C-8D27-8175FD9C3C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Jack</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>09/19/2020</t>
+  </si>
+  <si>
+    <t>Wesley</t>
+  </si>
+  <si>
+    <t>"158760334335672320"</t>
+  </si>
+  <si>
+    <t>11/12/2020</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>"814697817989185537"</t>
   </si>
 </sst>
 </file>
@@ -180,12 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FA76DC-CD61-4D4C-9E50-AB513A220CF7}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +696,34 @@
         <v>24</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3">
+        <v>43962</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>